<commit_message>
[GEN MCU] 실구매 부품으로 update
</commit_message>
<xml_diff>
--- a/1_LF_Generator_MCU/1_Schematic/V1.0/Plasma_LF_Gen_MCU_BOM V1.0.xlsx
+++ b/1_LF_Generator_MCU/1_Schematic/V1.0/Plasma_LF_Gen_MCU_BOM V1.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SWEND066\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Work\20171211_Femto_LF Gen\0_GitHub_Data_LF\1_LF_Generator_MCU\1_Schematic\V1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Plasma_LF_Gen_MCU_SCH_V1.0" sheetId="1" r:id="rId1"/>
+    <sheet name="전체비용" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Plasma_LF_Gen_MCU_SCH_V1.0!$B$4:$L$4</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="206">
   <si>
     <t>No</t>
   </si>
@@ -333,24 +334,12 @@
     <t>2.4x2.12</t>
   </si>
   <si>
-    <t>54102-S08-05</t>
-  </si>
-  <si>
-    <t>FCI</t>
-  </si>
-  <si>
-    <t>2.54mm pitch 10-pin(2x5) Header Post=5.84mm Tail=3.05mm</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
     <t>5.84mm</t>
   </si>
   <si>
-    <t>A1-10PA-2.54DSA</t>
-  </si>
-  <si>
     <t>12.7x4.83</t>
   </si>
   <si>
@@ -372,15 +361,6 @@
     <t>4.25x3.2</t>
   </si>
   <si>
-    <t>HEADER_20X2</t>
-  </si>
-  <si>
-    <t>57102-G06-20LF</t>
-  </si>
-  <si>
-    <t>2.00mm pitch 40-pin(20x2) Header Post=4mm Tail=2.5mm</t>
-  </si>
-  <si>
     <t>J9,J10</t>
   </si>
   <si>
@@ -412,9 +392,6 @@
   </si>
   <si>
     <t>ABS07-32.768KHZ</t>
-  </si>
-  <si>
-    <t>ABS07-120-32.768KHz-T</t>
   </si>
   <si>
     <t>ABRACON</t>
@@ -510,7 +487,167 @@
     <t>P007092561</t>
   </si>
   <si>
-    <t>P007602652</t>
+    <t>Sample</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>작업내용</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Point</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>단가</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>금액</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMD</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>부자재</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>이윤</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>소계</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>작업내용</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>수량</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>단가</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>금액</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Metal mask</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>부품비</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>합계</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 제작비용</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMD는 sample build 견적으로 양산시 재견적 확인 필요함</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>작업내용</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Point</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>단가</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>금액</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>수삽</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>부자재</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>수량</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>수삽</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>부품비</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>합계</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>제이엘텍 - Sample build 견적</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>작업내용</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Point</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>단가</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>금액</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>이윤</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>수량</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>P005675364</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>P005666489</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
@@ -518,23 +655,47 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>P005013055</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>P000096310</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">P005745361 </t>
+    <t>P007366368</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>P008255995</t>
+    <t>ABS07AIG-32.768KHZ-6-D-T</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>Sample</t>
+    <t>P008215485</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.00mm pitch 40-pin(20x2) Header L=8.8mm(1-molding)</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anyvendor</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.54mm pitch 10-pin(2x5) Header L=11.5mm(1-molding)</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>HEADER_2.54mm_2x5</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>HEADER_2.0mm_2x20</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABS07-32.768KHZ</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABS07AIG-32.768KHZ-6-D-T</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -542,11 +703,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0\ &quot;%&quot;"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -722,8 +884,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -921,8 +1090,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1272,6 +1447,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1403,12 +1623,12 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1454,9 +1674,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1544,7 +1761,71 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="24" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="18" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="18" fillId="33" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="18" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="18" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1874,34 +2155,35 @@
   <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.875" customWidth="1"/>
     <col min="2" max="2" width="6.625" customWidth="1"/>
-    <col min="3" max="4" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="60.25" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="27.25" customWidth="1"/>
+    <col min="9" max="9" width="27.25" hidden="1" customWidth="1"/>
     <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="23.125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16" customWidth="1"/>
-    <col min="21" max="21" width="9" style="26"/>
+    <col min="21" max="21" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="U1" s="27"/>
+        <v>133</v>
+      </c>
+      <c r="U1" s="26"/>
     </row>
     <row r="3" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O3" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="P3">
         <v>10</v>
@@ -1945,38 +2227,38 @@
         <v>10</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="O4" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="U4" s="30" t="s">
         <v>145</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="T4" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="U4" s="31" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="21">
         <v>1</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -2016,19 +2298,19 @@
         <f>H5*M5</f>
         <v>20</v>
       </c>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="32"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="31"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <v>2</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -2068,19 +2350,19 @@
         <f t="shared" ref="N6:N30" si="0">H6*M6</f>
         <v>20</v>
       </c>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="20"/>
-      <c r="U6" s="30"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="29"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="17">
         <v>3</v>
       </c>
       <c r="C7" s="14" t="s">
@@ -2120,19 +2402,19 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="30"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="29"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="17">
         <v>4</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -2172,19 +2454,19 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="30"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="29"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="17">
         <v>5</v>
       </c>
       <c r="C9" s="14" t="s">
@@ -2224,19 +2506,19 @@
         <f t="shared" si="0"/>
         <v>420</v>
       </c>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="20"/>
-      <c r="U9" s="30"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="29"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="17">
         <v>6</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -2276,19 +2558,19 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="20"/>
-      <c r="U10" s="30"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="29"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="17">
         <v>7</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -2328,19 +2610,19 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="20"/>
-      <c r="U11" s="30"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="29"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="17">
         <v>8</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -2380,19 +2662,19 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="20"/>
-      <c r="U12" s="30"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="29"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="17">
         <v>9</v>
       </c>
       <c r="C13" s="14" t="s">
@@ -2432,65 +2714,65 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="20"/>
-      <c r="U13" s="30"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="29"/>
     </row>
     <row r="14" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="22">
         <v>10</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="15">
         <v>4</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="16" t="s">
+      <c r="K14" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="L14" s="16" t="s">
+      <c r="L14" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="M14" s="16">
+      <c r="M14" s="15">
         <v>10</v>
       </c>
-      <c r="N14" s="16">
+      <c r="N14" s="15">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="29"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="28"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -2544,23 +2826,23 @@
       <c r="Q15" s="3">
         <v>1</v>
       </c>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="42" t="s">
-        <v>151</v>
+      <c r="R15" s="74"/>
+      <c r="S15" s="74"/>
+      <c r="T15" s="41" t="s">
+        <v>143</v>
       </c>
       <c r="U15" s="3">
         <v>100</v>
       </c>
       <c r="V15" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="17">
         <v>12</v>
       </c>
       <c r="C16" s="14" t="s">
@@ -2608,23 +2890,23 @@
       <c r="Q16" s="14">
         <v>10</v>
       </c>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="42" t="s">
-        <v>154</v>
-      </c>
-      <c r="U16" s="28">
+      <c r="R16" s="75"/>
+      <c r="S16" s="75"/>
+      <c r="T16" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="U16" s="27">
         <v>40</v>
       </c>
-      <c r="V16" s="33" t="s">
-        <v>152</v>
+      <c r="V16" s="32" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="17">
         <v>13</v>
       </c>
       <c r="C17" s="14" t="s">
@@ -2672,23 +2954,23 @@
       <c r="Q17" s="14">
         <v>10</v>
       </c>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
+      <c r="R17" s="75"/>
+      <c r="S17" s="75"/>
       <c r="T17" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="U17" s="28">
+        <v>147</v>
+      </c>
+      <c r="U17" s="27">
         <v>20</v>
       </c>
-      <c r="V17" s="34" t="s">
-        <v>152</v>
+      <c r="V17" s="33" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="17">
         <v>14</v>
       </c>
       <c r="C18" s="14" t="s">
@@ -2736,23 +3018,23 @@
       <c r="Q18" s="14">
         <v>10</v>
       </c>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
+      <c r="R18" s="75"/>
+      <c r="S18" s="75"/>
       <c r="T18" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="U18" s="28">
+        <v>148</v>
+      </c>
+      <c r="U18" s="27">
         <v>40</v>
       </c>
-      <c r="V18" s="35" t="s">
-        <v>152</v>
+      <c r="V18" s="34" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="17">
         <v>15</v>
       </c>
       <c r="C19" s="14" t="s">
@@ -2798,23 +3080,23 @@
       <c r="Q19" s="14">
         <v>1</v>
       </c>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="44" t="s">
-        <v>157</v>
-      </c>
-      <c r="U19" s="28">
+      <c r="R19" s="75"/>
+      <c r="S19" s="75"/>
+      <c r="T19" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="U19" s="27">
         <v>120</v>
       </c>
       <c r="V19" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="17">
         <v>16</v>
       </c>
       <c r="C20" s="14" t="s">
@@ -2862,23 +3144,23 @@
       <c r="Q20" s="14">
         <v>1</v>
       </c>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="42" t="s">
-        <v>157</v>
-      </c>
-      <c r="U20" s="28">
+      <c r="R20" s="75"/>
+      <c r="S20" s="75"/>
+      <c r="T20" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="U20" s="27">
         <v>40</v>
       </c>
-      <c r="V20" s="36" t="s">
-        <v>152</v>
+      <c r="V20" s="35" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>17</v>
       </c>
       <c r="C21" s="14" t="s">
@@ -2926,23 +3208,23 @@
       <c r="Q21" s="14">
         <v>1</v>
       </c>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="42" t="s">
-        <v>159</v>
-      </c>
-      <c r="U21" s="28">
+      <c r="R21" s="75"/>
+      <c r="S21" s="75"/>
+      <c r="T21" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="U21" s="27">
         <v>60</v>
       </c>
-      <c r="V21" s="37" t="s">
-        <v>152</v>
+      <c r="V21" s="36" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="17">
         <v>18</v>
       </c>
       <c r="C22" s="14" t="s">
@@ -2990,63 +3272,65 @@
       <c r="Q22" s="14">
         <v>1</v>
       </c>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="42" t="s">
-        <v>160</v>
-      </c>
-      <c r="U22" s="28">
+      <c r="R22" s="75"/>
+      <c r="S22" s="75"/>
+      <c r="T22" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="U22" s="27">
         <v>40</v>
       </c>
-      <c r="V22" s="38" t="s">
-        <v>152</v>
+      <c r="V22" s="37" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="17">
         <v>19</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>105</v>
+      <c r="C23" s="76" t="s">
+        <v>202</v>
+      </c>
+      <c r="D23" s="76" t="s">
+        <v>202</v>
+      </c>
+      <c r="E23" s="76" t="s">
+        <v>200</v>
+      </c>
+      <c r="F23" s="76" t="s">
+        <v>202</v>
+      </c>
+      <c r="G23" s="76" t="s">
+        <v>201</v>
       </c>
       <c r="H23" s="14">
         <v>1</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="L23" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="M23" s="14">
-        <v>890</v>
+        <v>104</v>
+      </c>
+      <c r="L23" s="76" t="s">
+        <v>202</v>
+      </c>
+      <c r="M23" s="76">
+        <v>30</v>
       </c>
       <c r="N23" s="14">
         <f t="shared" si="0"/>
-        <v>890</v>
-      </c>
-      <c r="O23" s="14"/>
+        <v>30</v>
+      </c>
+      <c r="O23" s="14">
+        <v>30</v>
+      </c>
       <c r="P23" s="3">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -3054,49 +3338,54 @@
       <c r="Q23" s="14">
         <v>1</v>
       </c>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="45" t="s">
-        <v>161</v>
-      </c>
-      <c r="U23" s="28"/>
+      <c r="R23" s="75">
+        <v>10</v>
+      </c>
+      <c r="S23" s="75">
+        <f>O23*R23</f>
+        <v>300</v>
+      </c>
+      <c r="T23" s="73" t="s">
+        <v>193</v>
+      </c>
+      <c r="U23" s="27"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="17">
         <v>20</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H24" s="14">
         <v>1</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="L24" s="14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="M24" s="14">
         <v>50</v>
@@ -3105,7 +3394,9 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="O24" s="14"/>
+      <c r="O24" s="14">
+        <v>50</v>
+      </c>
       <c r="P24" s="3">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -3113,58 +3404,65 @@
       <c r="Q24" s="14">
         <v>100</v>
       </c>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="45" t="s">
-        <v>162</v>
-      </c>
-      <c r="U24" s="28"/>
+      <c r="R24" s="75">
+        <v>100</v>
+      </c>
+      <c r="S24" s="75">
+        <f>O24*R24</f>
+        <v>5000</v>
+      </c>
+      <c r="T24" s="73" t="s">
+        <v>194</v>
+      </c>
+      <c r="U24" s="27"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="17">
         <v>21</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>118</v>
+      <c r="C25" s="76" t="s">
+        <v>203</v>
+      </c>
+      <c r="D25" s="76" t="s">
+        <v>203</v>
+      </c>
+      <c r="E25" s="76" t="s">
+        <v>200</v>
+      </c>
+      <c r="F25" s="76" t="s">
+        <v>203</v>
+      </c>
+      <c r="G25" s="76" t="s">
+        <v>199</v>
       </c>
       <c r="H25" s="14">
         <v>2</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="K25" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="L25" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="M25" s="14">
-        <v>4180</v>
+        <v>113</v>
+      </c>
+      <c r="L25" s="76" t="s">
+        <v>203</v>
+      </c>
+      <c r="M25" s="76">
+        <v>290</v>
       </c>
       <c r="N25" s="14">
         <f t="shared" si="0"/>
-        <v>8360</v>
-      </c>
-      <c r="O25" s="14"/>
+        <v>580</v>
+      </c>
+      <c r="O25" s="14">
+        <v>290</v>
+      </c>
       <c r="P25" s="3">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -3172,49 +3470,54 @@
       <c r="Q25" s="14">
         <v>1</v>
       </c>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="45" t="s">
-        <v>163</v>
-      </c>
-      <c r="U25" s="28"/>
+      <c r="R25" s="75">
+        <v>20</v>
+      </c>
+      <c r="S25" s="75">
+        <f>O25*R25</f>
+        <v>5800</v>
+      </c>
+      <c r="T25" s="73" t="s">
+        <v>192</v>
+      </c>
+      <c r="U25" s="27"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="17">
         <v>22</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="H26" s="14">
         <v>1</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="L26" s="14" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="M26" s="14">
         <v>100</v>
@@ -3223,7 +3526,9 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="O26" s="14"/>
+      <c r="O26" s="14">
+        <v>100</v>
+      </c>
       <c r="P26" s="3">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -3231,58 +3536,65 @@
       <c r="Q26" s="14">
         <v>10</v>
       </c>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="U26" s="28"/>
+      <c r="R26" s="75">
+        <v>10</v>
+      </c>
+      <c r="S26" s="75">
+        <f>O26*R26</f>
+        <v>1000</v>
+      </c>
+      <c r="T26" s="73" t="s">
+        <v>195</v>
+      </c>
+      <c r="U26" s="27"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="17">
         <v>23</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>130</v>
+      <c r="C27" s="76" t="s">
+        <v>204</v>
+      </c>
+      <c r="D27" s="76" t="s">
+        <v>205</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>130</v>
+        <v>123</v>
+      </c>
+      <c r="F27" s="76" t="s">
+        <v>197</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="H27" s="14">
         <v>1</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="K27" s="14" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="L27" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="M27" s="14">
-        <v>840</v>
+        <v>122</v>
+      </c>
+      <c r="M27" s="76">
+        <v>430</v>
       </c>
       <c r="N27" s="14">
         <f t="shared" si="0"/>
-        <v>840</v>
-      </c>
-      <c r="O27" s="14"/>
+        <v>430</v>
+      </c>
+      <c r="O27" s="14">
+        <v>430</v>
+      </c>
       <c r="P27" s="3">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -3290,58 +3602,65 @@
       <c r="Q27" s="14">
         <v>1</v>
       </c>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="U27" s="28"/>
+      <c r="R27" s="75">
+        <v>10</v>
+      </c>
+      <c r="S27" s="75">
+        <f>O27*R27</f>
+        <v>4300</v>
+      </c>
+      <c r="T27" s="73" t="s">
+        <v>196</v>
+      </c>
+      <c r="U27" s="27"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="17">
         <v>24</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="H28" s="14">
         <v>1</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="M28" s="14">
-        <v>720</v>
+        <v>128</v>
+      </c>
+      <c r="M28" s="76">
+        <v>430</v>
       </c>
       <c r="N28" s="14">
         <f t="shared" si="0"/>
-        <v>720</v>
-      </c>
-      <c r="O28" s="14"/>
+        <v>430</v>
+      </c>
+      <c r="O28" s="14">
+        <v>430</v>
+      </c>
       <c r="P28" s="3">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -3349,128 +3668,137 @@
       <c r="Q28" s="14">
         <v>1</v>
       </c>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="45" t="s">
-        <v>166</v>
-      </c>
-      <c r="U28" s="28"/>
+      <c r="R28" s="75">
+        <v>10</v>
+      </c>
+      <c r="S28" s="75">
+        <f>O28*R28</f>
+        <v>4300</v>
+      </c>
+      <c r="T28" s="73" t="s">
+        <v>198</v>
+      </c>
+      <c r="U28" s="27"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="40">
+      <c r="B29" s="39">
         <v>25</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="41" t="s">
+      <c r="D29" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="41" t="s">
+      <c r="E29" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="41" t="s">
+      <c r="F29" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="41" t="s">
+      <c r="G29" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="41">
+      <c r="H29" s="40">
         <v>3</v>
       </c>
-      <c r="I29" s="41" t="s">
+      <c r="I29" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="J29" s="41" t="s">
+      <c r="J29" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="K29" s="41" t="s">
+      <c r="K29" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="L29" s="41" t="s">
+      <c r="L29" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="M29" s="41">
+      <c r="M29" s="40">
         <v>0</v>
       </c>
-      <c r="N29" s="41">
+      <c r="N29" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O29" s="41"/>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="41"/>
-      <c r="R29" s="41"/>
-      <c r="S29" s="41"/>
-      <c r="T29" s="42"/>
-      <c r="U29" s="41"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="40"/>
+      <c r="R29" s="40"/>
+      <c r="S29" s="40"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="40"/>
     </row>
     <row r="30" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="40">
+      <c r="B30" s="39">
         <v>26</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="39" t="s">
+      <c r="D30" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="39" t="s">
+      <c r="E30" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="F30" s="39" t="s">
+      <c r="F30" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="39" t="s">
+      <c r="G30" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="H30" s="39">
+      <c r="H30" s="38">
         <v>6</v>
       </c>
-      <c r="I30" s="39" t="s">
+      <c r="I30" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="J30" s="39" t="s">
+      <c r="J30" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="K30" s="39" t="s">
+      <c r="K30" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="L30" s="39" t="s">
+      <c r="L30" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="M30" s="39">
+      <c r="M30" s="38">
         <v>0</v>
       </c>
-      <c r="N30" s="39">
+      <c r="N30" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O30" s="39"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="39"/>
-      <c r="R30" s="39"/>
-      <c r="S30" s="39"/>
-      <c r="T30" s="43"/>
-      <c r="U30" s="39"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38"/>
+      <c r="R30" s="38"/>
+      <c r="S30" s="38"/>
+      <c r="T30" s="42"/>
+      <c r="U30" s="38"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H31" s="4">
+        <f>SUM(H5:H28)</f>
+        <v>52</v>
+      </c>
       <c r="N31" s="4">
         <f>SUM(N5:N30)</f>
-        <v>17320</v>
+        <v>7980</v>
       </c>
     </row>
     <row r="32" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="U32" s="27"/>
+        <v>134</v>
+      </c>
+      <c r="U32" s="26"/>
     </row>
   </sheetData>
   <autoFilter ref="B4:L4"/>
@@ -3478,4 +3806,444 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="4.375" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J3" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="O3" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+    </row>
+    <row r="4" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="J4" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="K4" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="L4" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="M4" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="O4" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="P4" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q4" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="R4" s="46" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C5" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="48">
+        <v>52</v>
+      </c>
+      <c r="E5" s="48">
+        <v>670</v>
+      </c>
+      <c r="F5" s="49">
+        <f>D5*E5</f>
+        <v>34840</v>
+      </c>
+      <c r="J5" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="K5" s="48">
+        <v>169</v>
+      </c>
+      <c r="L5" s="48">
+        <v>500</v>
+      </c>
+      <c r="M5" s="49">
+        <f>K5*L5</f>
+        <v>84500</v>
+      </c>
+      <c r="O5" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="P5" s="48">
+        <v>169</v>
+      </c>
+      <c r="Q5" s="48">
+        <v>630</v>
+      </c>
+      <c r="R5" s="49">
+        <f>P5*Q5</f>
+        <v>106470</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C6" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="51">
+        <v>15</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" s="53">
+        <f>F5*D6/100</f>
+        <v>5226</v>
+      </c>
+      <c r="J6" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="K6" s="51">
+        <v>15</v>
+      </c>
+      <c r="L6" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="M6" s="53">
+        <f>M5*K6/100</f>
+        <v>12675</v>
+      </c>
+      <c r="O6" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="P6" s="51">
+        <v>15</v>
+      </c>
+      <c r="Q6" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="R6" s="53">
+        <f>R5*P6/100</f>
+        <v>15970.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="55">
+        <v>15</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" s="57">
+        <f>F5*D7/100</f>
+        <v>5226</v>
+      </c>
+      <c r="J7" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="K7" s="55">
+        <v>0</v>
+      </c>
+      <c r="L7" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="M7" s="57">
+        <f>M5*K7/100</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="54" t="s">
+        <v>190</v>
+      </c>
+      <c r="P7" s="55">
+        <v>15</v>
+      </c>
+      <c r="Q7" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="R7" s="57">
+        <f>R5*P7/100</f>
+        <v>15970.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="58">
+        <f>SUM(F5:F7)</f>
+        <v>45292</v>
+      </c>
+      <c r="J8" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="K8" s="70"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="58">
+        <f>SUM(M5:M7)</f>
+        <v>97175</v>
+      </c>
+      <c r="O8" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="P8" s="70"/>
+      <c r="Q8" s="70"/>
+      <c r="R8" s="58">
+        <f>SUM(R5:R7)</f>
+        <v>138411</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="59"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="60"/>
+    </row>
+    <row r="10" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="61" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="F10" s="64" t="s">
+        <v>166</v>
+      </c>
+      <c r="J10" s="61" t="s">
+        <v>174</v>
+      </c>
+      <c r="K10" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="L10" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="M10" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="O10" s="61" t="s">
+        <v>185</v>
+      </c>
+      <c r="P10" s="62" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q10" s="63" t="s">
+        <v>187</v>
+      </c>
+      <c r="R10" s="64" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C11" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="48">
+        <v>100</v>
+      </c>
+      <c r="E11" s="48">
+        <f>F8</f>
+        <v>45292</v>
+      </c>
+      <c r="F11" s="65">
+        <f>D11*E11</f>
+        <v>4529200</v>
+      </c>
+      <c r="J11" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="K11" s="48">
+        <v>4</v>
+      </c>
+      <c r="L11" s="48">
+        <f>M8</f>
+        <v>97175</v>
+      </c>
+      <c r="M11" s="65">
+        <f>K11*L11</f>
+        <v>388700</v>
+      </c>
+      <c r="O11" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="P11" s="48">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="48">
+        <f>R8</f>
+        <v>138411</v>
+      </c>
+      <c r="R11" s="65">
+        <f>P11*Q11</f>
+        <v>553644</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="66">
+        <v>1</v>
+      </c>
+      <c r="E12" s="66">
+        <v>110000</v>
+      </c>
+      <c r="F12" s="67">
+        <f>D12*E12</f>
+        <v>110000</v>
+      </c>
+      <c r="J12" s="54" t="s">
+        <v>182</v>
+      </c>
+      <c r="K12" s="66">
+        <v>4</v>
+      </c>
+      <c r="L12" s="66">
+        <v>0</v>
+      </c>
+      <c r="M12" s="67">
+        <f>K12*L12</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="54" t="s">
+        <v>182</v>
+      </c>
+      <c r="P12" s="66">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="66">
+        <v>0</v>
+      </c>
+      <c r="R12" s="67">
+        <f>P12*Q12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="66">
+        <v>100</v>
+      </c>
+      <c r="E13" s="66">
+        <f>Plasma_LF_Gen_MCU_SCH_V1.0!N31</f>
+        <v>7980</v>
+      </c>
+      <c r="F13" s="67">
+        <f>D13*E13</f>
+        <v>798000</v>
+      </c>
+      <c r="J13" s="69" t="s">
+        <v>183</v>
+      </c>
+      <c r="K13" s="70"/>
+      <c r="L13" s="71">
+        <f>M11</f>
+        <v>388700</v>
+      </c>
+      <c r="M13" s="72"/>
+      <c r="O13" s="69" t="s">
+        <v>183</v>
+      </c>
+      <c r="P13" s="70"/>
+      <c r="Q13" s="71">
+        <f>R11</f>
+        <v>553644</v>
+      </c>
+      <c r="R13" s="72"/>
+    </row>
+    <row r="14" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="69" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" s="70"/>
+      <c r="E14" s="71">
+        <f>SUM(F11:F13)</f>
+        <v>5437200</v>
+      </c>
+      <c r="F14" s="72"/>
+    </row>
+    <row r="15" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="69" t="s">
+        <v>171</v>
+      </c>
+      <c r="D16" s="70"/>
+      <c r="E16" s="71">
+        <f>E14/D11</f>
+        <v>54372</v>
+      </c>
+      <c r="F16" s="72"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+  </mergeCells>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[GEN MCU] Soldering check
</commit_message>
<xml_diff>
--- a/1_LF_Generator_MCU/1_Schematic/V1.0/Plasma_LF_Gen_MCU_BOM V1.0.xlsx
+++ b/1_LF_Generator_MCU/1_Schematic/V1.0/Plasma_LF_Gen_MCU_BOM V1.0.xlsx
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Plasma_LF_Gen_MCU_SCH_V1.0!$B$4:$L$4</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -173,9 +173,6 @@
     <t>RES SMD 10K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t>R6,R7,R16,R21</t>
-  </si>
-  <si>
     <t>WR04X000PTL</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>LQM2HPZ2R2MG0</t>
   </si>
   <si>
-    <t>Murata</t>
-  </si>
-  <si>
     <t>FIXED IND 2.2UH 1.3A 80 MOHM SMD, SRF 40MHz</t>
   </si>
   <si>
@@ -257,9 +251,6 @@
     <t>Backlight LED SMD 1608 Green</t>
   </si>
   <si>
-    <t>LED5</t>
-  </si>
-  <si>
     <t>0.6mm</t>
   </si>
   <si>
@@ -267,9 +258,6 @@
   </si>
   <si>
     <t>Diodes</t>
-  </si>
-  <si>
-    <t>D1,D2,D3,D4,D5</t>
   </si>
   <si>
     <t>1.05mm</t>
@@ -691,6 +679,66 @@
   </si>
   <si>
     <t>ABS07AIG-32.768KHZ-6-D-T</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Murata</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R6,R7,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R16,R21</t>
+    </r>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>D1,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,D3,D4,D5</t>
+    </r>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED5</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -703,7 +751,7 @@
     <numFmt numFmtId="176" formatCode="0\ &quot;%&quot;"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -881,6 +929,29 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -1623,7 +1694,7 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1822,6 +1893,15 @@
     </xf>
     <xf numFmtId="41" fontId="18" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="26" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -2139,7 +2219,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2150,7 +2230,7 @@
   <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2163,8 +2243,8 @@
     <col min="6" max="6" width="23.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="60.25" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="27.25" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="27.25" customWidth="1"/>
+    <col min="10" max="11" width="9" customWidth="1"/>
     <col min="12" max="12" width="23.125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16" customWidth="1"/>
     <col min="21" max="21" width="9" style="25"/>
@@ -2172,13 +2252,13 @@
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="U1" s="26"/>
     </row>
     <row r="3" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="P3">
         <v>10</v>
@@ -2222,31 +2302,31 @@
         <v>10</v>
       </c>
       <c r="M4" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q4" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="R4" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="S4" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="T4" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="Q4" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="S4" s="11" t="s">
+      <c r="U4" s="30" t="s">
         <v>141</v>
-      </c>
-      <c r="T4" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="U4" s="30" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -2526,16 +2606,16 @@
         <v>43</v>
       </c>
       <c r="F10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="H10" s="14">
         <v>5</v>
       </c>
-      <c r="I10" s="14" t="s">
-        <v>54</v>
+      <c r="I10" s="72" t="s">
+        <v>53</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>20</v>
@@ -2578,16 +2658,16 @@
         <v>43</v>
       </c>
       <c r="F11" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="H11" s="14">
         <v>2</v>
       </c>
-      <c r="I11" s="14" t="s">
-        <v>60</v>
+      <c r="I11" s="72" t="s">
+        <v>59</v>
       </c>
       <c r="J11" s="14" t="s">
         <v>20</v>
@@ -2638,7 +2718,7 @@
       <c r="H12" s="14">
         <v>5</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="72" t="s">
         <v>46</v>
       </c>
       <c r="J12" s="14" t="s">
@@ -2676,22 +2756,22 @@
         <v>42</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>43</v>
       </c>
       <c r="F13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>58</v>
       </c>
       <c r="H13" s="14">
         <v>1</v>
       </c>
-      <c r="I13" s="14" t="s">
-        <v>59</v>
+      <c r="I13" s="72" t="s">
+        <v>58</v>
       </c>
       <c r="J13" s="14" t="s">
         <v>20</v>
@@ -2742,8 +2822,8 @@
       <c r="H14" s="15">
         <v>4</v>
       </c>
-      <c r="I14" s="15" t="s">
-        <v>51</v>
+      <c r="I14" s="79" t="s">
+        <v>203</v>
       </c>
       <c r="J14" s="15" t="s">
         <v>20</v>
@@ -2777,34 +2857,34 @@
         <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="H15" s="3">
         <v>1</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J15" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="K15" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M15" s="3">
         <v>430</v>
@@ -2824,13 +2904,13 @@
       <c r="R15" s="70"/>
       <c r="S15" s="70"/>
       <c r="T15" s="41" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="U15" s="3">
         <v>100</v>
       </c>
       <c r="V15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
@@ -2841,34 +2921,34 @@
         <v>12</v>
       </c>
       <c r="C16" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="F16" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="14" t="s">
         <v>68</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>70</v>
       </c>
       <c r="H16" s="14">
         <v>2</v>
       </c>
-      <c r="I16" s="14" t="s">
-        <v>71</v>
+      <c r="I16" s="72" t="s">
+        <v>69</v>
       </c>
       <c r="J16" s="14" t="s">
         <v>37</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L16" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M16" s="14">
         <v>20</v>
@@ -2888,13 +2968,13 @@
       <c r="R16" s="71"/>
       <c r="S16" s="71"/>
       <c r="T16" s="41" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="U16" s="27">
         <v>40</v>
       </c>
       <c r="V16" s="32" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
@@ -2905,34 +2985,34 @@
         <v>13</v>
       </c>
       <c r="C17" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>69</v>
-      </c>
       <c r="F17" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H17" s="14">
         <v>2</v>
       </c>
-      <c r="I17" s="14" t="s">
-        <v>75</v>
+      <c r="I17" s="72" t="s">
+        <v>73</v>
       </c>
       <c r="J17" s="14" t="s">
         <v>37</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L17" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M17" s="14">
         <v>30</v>
@@ -2952,13 +3032,13 @@
       <c r="R17" s="71"/>
       <c r="S17" s="71"/>
       <c r="T17" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="U17" s="27">
         <v>20</v>
       </c>
       <c r="V17" s="33" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
@@ -2969,34 +3049,34 @@
         <v>14</v>
       </c>
       <c r="C18" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>69</v>
-      </c>
       <c r="F18" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H18" s="14">
         <v>1</v>
       </c>
-      <c r="I18" s="14" t="s">
-        <v>79</v>
+      <c r="I18" s="72" t="s">
+        <v>205</v>
       </c>
       <c r="J18" s="14" t="s">
         <v>37</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L18" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M18" s="14">
         <v>20</v>
@@ -3016,13 +3096,13 @@
       <c r="R18" s="71"/>
       <c r="S18" s="71"/>
       <c r="T18" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="U18" s="27">
         <v>40</v>
       </c>
       <c r="V18" s="34" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
@@ -3033,32 +3113,32 @@
         <v>15</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14">
         <v>5</v>
       </c>
-      <c r="I19" s="14" t="s">
-        <v>83</v>
+      <c r="I19" s="78" t="s">
+        <v>204</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="M19" s="14">
         <v>60</v>
@@ -3078,13 +3158,13 @@
       <c r="R19" s="71"/>
       <c r="S19" s="71"/>
       <c r="T19" s="43" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="U19" s="27">
         <v>120</v>
       </c>
       <c r="V19" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
@@ -3095,34 +3175,34 @@
         <v>16</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H20" s="14">
         <v>1</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="M20" s="14">
         <v>2760</v>
@@ -3142,13 +3222,13 @@
       <c r="R20" s="71"/>
       <c r="S20" s="71"/>
       <c r="T20" s="41" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="U20" s="27">
         <v>40</v>
       </c>
       <c r="V20" s="35" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
@@ -3159,34 +3239,34 @@
         <v>17</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H21" s="14">
         <v>1</v>
       </c>
-      <c r="I21" s="14" t="s">
-        <v>95</v>
+      <c r="I21" s="72" t="s">
+        <v>91</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="M21" s="14">
         <v>1170</v>
@@ -3206,13 +3286,13 @@
       <c r="R21" s="71"/>
       <c r="S21" s="71"/>
       <c r="T21" s="41" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="U21" s="27">
         <v>60</v>
       </c>
       <c r="V21" s="36" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
@@ -3223,34 +3303,34 @@
         <v>18</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H22" s="14">
         <v>1</v>
       </c>
-      <c r="I22" s="14" t="s">
-        <v>100</v>
+      <c r="I22" s="72" t="s">
+        <v>96</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="L22" s="14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="M22" s="14">
         <v>870</v>
@@ -3270,13 +3350,13 @@
       <c r="R22" s="71"/>
       <c r="S22" s="71"/>
       <c r="T22" s="41" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="U22" s="27">
         <v>40</v>
       </c>
       <c r="V22" s="37" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
@@ -3287,34 +3367,34 @@
         <v>19</v>
       </c>
       <c r="C23" s="72" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D23" s="72" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E23" s="72" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F23" s="72" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G23" s="72" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H23" s="14">
         <v>1</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L23" s="72" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M23" s="72">
         <v>30</v>
@@ -3341,7 +3421,7 @@
         <v>300</v>
       </c>
       <c r="T23" s="69" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="U23" s="27"/>
     </row>
@@ -3353,34 +3433,34 @@
         <v>20</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H24" s="14">
         <v>1</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L24" s="14" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="M24" s="14">
         <v>50</v>
@@ -3407,7 +3487,7 @@
         <v>5000</v>
       </c>
       <c r="T24" s="69" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="U24" s="27"/>
     </row>
@@ -3419,34 +3499,34 @@
         <v>21</v>
       </c>
       <c r="C25" s="72" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D25" s="72" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E25" s="72" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F25" s="72" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G25" s="72" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H25" s="14">
         <v>2</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K25" s="14" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L25" s="72" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="M25" s="72">
         <v>290</v>
@@ -3473,7 +3553,7 @@
         <v>5800</v>
       </c>
       <c r="T25" s="69" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="U25" s="27"/>
     </row>
@@ -3485,34 +3565,34 @@
         <v>22</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H26" s="14">
         <v>1</v>
       </c>
-      <c r="I26" s="14" t="s">
-        <v>119</v>
+      <c r="I26" s="72" t="s">
+        <v>115</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="L26" s="14" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M26" s="14">
         <v>100</v>
@@ -3539,7 +3619,7 @@
         <v>1000</v>
       </c>
       <c r="T26" s="69" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="U26" s="27"/>
     </row>
@@ -3551,34 +3631,34 @@
         <v>23</v>
       </c>
       <c r="C27" s="72" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D27" s="72" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F27" s="72" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H27" s="14">
         <v>1</v>
       </c>
-      <c r="I27" s="14" t="s">
-        <v>125</v>
+      <c r="I27" s="40" t="s">
+        <v>121</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K27" s="14" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="L27" s="14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="M27" s="72">
         <v>430</v>
@@ -3605,7 +3685,7 @@
         <v>4300</v>
       </c>
       <c r="T27" s="69" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="U27" s="27"/>
     </row>
@@ -3617,34 +3697,34 @@
         <v>24</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H28" s="14">
         <v>1</v>
       </c>
-      <c r="I28" s="14" t="s">
-        <v>130</v>
+      <c r="I28" s="40" t="s">
+        <v>126</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="M28" s="72">
         <v>430</v>
@@ -3671,7 +3751,7 @@
         <v>4300</v>
       </c>
       <c r="T28" s="69" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="U28" s="27"/>
     </row>
@@ -3753,7 +3833,7 @@
         <v>6</v>
       </c>
       <c r="I30" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J30" s="38" t="s">
         <v>20</v>
@@ -3791,7 +3871,7 @@
     </row>
     <row r="32" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="U32" s="26"/>
     </row>
@@ -3820,21 +3900,21 @@
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="J3" s="59" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K3" s="68"/>
       <c r="L3" s="68"/>
       <c r="M3" s="68"/>
       <c r="O3" s="59" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="P3" s="68"/>
       <c r="Q3" s="68"/>
@@ -3842,45 +3922,45 @@
     </row>
     <row r="4" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="44" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F4" s="46" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J4" s="44" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K4" s="45" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="L4" s="45" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="M4" s="46" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="O4" s="44" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="P4" s="45" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="Q4" s="45" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="R4" s="46" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C5" s="47" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D5" s="48">
         <v>52</v>
@@ -3893,7 +3973,7 @@
         <v>34840</v>
       </c>
       <c r="J5" s="47" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K5" s="48">
         <v>169</v>
@@ -3906,7 +3986,7 @@
         <v>84500</v>
       </c>
       <c r="O5" s="47" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="P5" s="48">
         <v>169</v>
@@ -3921,39 +4001,39 @@
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C6" s="50" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D6" s="51">
         <v>15</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F6" s="53">
         <f>F5*D6/100</f>
         <v>5226</v>
       </c>
       <c r="J6" s="50" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K6" s="51">
         <v>15</v>
       </c>
       <c r="L6" s="52" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="M6" s="53">
         <f>M5*K6/100</f>
         <v>12675</v>
       </c>
       <c r="O6" s="50" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P6" s="51">
         <v>15</v>
       </c>
       <c r="Q6" s="52" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="R6" s="53">
         <f>R5*P6/100</f>
@@ -3962,39 +4042,39 @@
     </row>
     <row r="7" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="54" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D7" s="55">
         <v>15</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F7" s="57">
         <f>F5*D7/100</f>
         <v>5226</v>
       </c>
       <c r="J7" s="54" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K7" s="55">
         <v>0</v>
       </c>
       <c r="L7" s="56" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="M7" s="57">
         <f>M5*K7/100</f>
         <v>0</v>
       </c>
       <c r="O7" s="54" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="P7" s="55">
         <v>15</v>
       </c>
       <c r="Q7" s="56" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="R7" s="57">
         <f>R5*P7/100</f>
@@ -4003,7 +4083,7 @@
     </row>
     <row r="8" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="73" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D8" s="74"/>
       <c r="E8" s="74"/>
@@ -4012,7 +4092,7 @@
         <v>45292</v>
       </c>
       <c r="J8" s="73" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="K8" s="74"/>
       <c r="L8" s="74"/>
@@ -4021,7 +4101,7 @@
         <v>97175</v>
       </c>
       <c r="O8" s="73" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="P8" s="74"/>
       <c r="Q8" s="74"/>
@@ -4046,45 +4126,45 @@
     </row>
     <row r="10" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="61" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D10" s="62" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E10" s="63" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F10" s="64" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J10" s="61" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K10" s="62" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="L10" s="63" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="M10" s="64" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="O10" s="61" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="P10" s="62" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="Q10" s="63" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="R10" s="64" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C11" s="47" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D11" s="48">
         <v>100</v>
@@ -4098,7 +4178,7 @@
         <v>4529200</v>
       </c>
       <c r="J11" s="47" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="K11" s="48">
         <v>4</v>
@@ -4112,7 +4192,7 @@
         <v>388700</v>
       </c>
       <c r="O11" s="47" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="P11" s="48">
         <v>4</v>
@@ -4128,7 +4208,7 @@
     </row>
     <row r="12" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="54" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D12" s="66">
         <v>1</v>
@@ -4141,7 +4221,7 @@
         <v>110000</v>
       </c>
       <c r="J12" s="54" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="K12" s="66">
         <v>4</v>
@@ -4154,7 +4234,7 @@
         <v>0</v>
       </c>
       <c r="O12" s="54" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="P12" s="66">
         <v>4</v>
@@ -4169,7 +4249,7 @@
     </row>
     <row r="13" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="54" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D13" s="66">
         <v>100</v>
@@ -4183,7 +4263,7 @@
         <v>798000</v>
       </c>
       <c r="J13" s="73" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K13" s="74"/>
       <c r="L13" s="75">
@@ -4192,7 +4272,7 @@
       </c>
       <c r="M13" s="76"/>
       <c r="O13" s="73" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="P13" s="74"/>
       <c r="Q13" s="75">
@@ -4203,7 +4283,7 @@
     </row>
     <row r="14" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="73" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D14" s="74"/>
       <c r="E14" s="75">
@@ -4215,7 +4295,7 @@
     <row r="15" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="73" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D16" s="74"/>
       <c r="E16" s="75">
@@ -4226,17 +4306,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="O13:P13"/>
     <mergeCell ref="Q13:R13"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[GEN MCU] Sample 제작
</commit_message>
<xml_diff>
--- a/1_LF_Generator_MCU/1_Schematic/V1.0/Plasma_LF_Gen_MCU_BOM V1.0.xlsx
+++ b/1_LF_Generator_MCU/1_Schematic/V1.0/Plasma_LF_Gen_MCU_BOM V1.0.xlsx
@@ -182,9 +182,6 @@
     <t>R8,R9,R10,R13,R14</t>
   </si>
   <si>
-    <t>R11,R12,R17,R18,R22,R23</t>
-  </si>
-  <si>
     <t>4.7K</t>
   </si>
   <si>
@@ -686,16 +683,20 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
+    <t>LED5</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>R7,R11,R12,R17,R18,R22,R23</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>R6,R16,R21</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R6,R7,</t>
+      <t>D1,</t>
     </r>
     <r>
       <rPr>
@@ -705,40 +706,8 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>R16,R21</t>
+      <t>D2,D3,D4,D5</t>
     </r>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>D1,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,D3,D4,D5</t>
-    </r>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>LED5</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -751,7 +720,7 @@
     <numFmt numFmtId="176" formatCode="0\ &quot;%&quot;"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -936,7 +905,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -945,15 +913,7 @@
     <font>
       <sz val="11"/>
       <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
+      <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -1694,7 +1654,7 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1879,9 +1839,6 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1894,13 +1851,19 @@
     <xf numFmtId="41" fontId="18" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="26" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2219,7 +2182,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2230,7 +2193,7 @@
   <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2252,13 +2215,13 @@
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U1" s="26"/>
     </row>
     <row r="3" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P3">
         <v>10</v>
@@ -2302,31 +2265,31 @@
         <v>10</v>
       </c>
       <c r="M4" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="N4" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="P4" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="Q4" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="R4" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="S4" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="S4" s="11" t="s">
+      <c r="T4" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="T4" s="12" t="s">
-        <v>138</v>
-      </c>
       <c r="U4" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -2440,37 +2403,37 @@
       <c r="B7" s="17">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="76">
         <v>7</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="L7" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="76">
         <v>10</v>
       </c>
       <c r="N7" s="14">
@@ -2492,37 +2455,37 @@
       <c r="B8" s="17">
         <v>4</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="76">
         <v>1</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="76">
         <v>10</v>
       </c>
       <c r="N8" s="14">
@@ -2544,37 +2507,37 @@
       <c r="B9" s="17">
         <v>5</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="76">
         <v>2</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="L9" s="14" t="s">
+      <c r="L9" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="76">
         <v>210</v>
       </c>
       <c r="N9" s="14">
@@ -2596,37 +2559,37 @@
       <c r="B10" s="17">
         <v>6</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="76">
         <v>0</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="76">
         <v>5</v>
       </c>
-      <c r="I10" s="72" t="s">
+      <c r="I10" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="14" t="s">
+      <c r="L10" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="76">
         <v>10</v>
       </c>
       <c r="N10" s="14">
@@ -2648,37 +2611,37 @@
       <c r="B11" s="17">
         <v>7</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="76">
         <v>100</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="76">
         <v>2</v>
       </c>
-      <c r="I11" s="72" t="s">
-        <v>59</v>
-      </c>
-      <c r="J11" s="14" t="s">
+      <c r="I11" s="76" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="K11" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="14" t="s">
+      <c r="L11" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11" s="76">
         <v>10</v>
       </c>
       <c r="N11" s="14">
@@ -2700,37 +2663,37 @@
       <c r="B12" s="17">
         <v>8</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="76">
         <v>470</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="76">
         <v>5</v>
       </c>
-      <c r="I12" s="72" t="s">
+      <c r="I12" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="K12" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="L12" s="14" t="s">
+      <c r="L12" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="M12" s="14">
+      <c r="M12" s="76">
         <v>10</v>
       </c>
       <c r="N12" s="14">
@@ -2752,37 +2715,37 @@
       <c r="B13" s="17">
         <v>9</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="14" t="s">
+      <c r="G13" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="H13" s="76">
+        <v>1</v>
+      </c>
+      <c r="I13" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="14">
-        <v>1</v>
-      </c>
-      <c r="I13" s="72" t="s">
-        <v>58</v>
-      </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="K13" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="L13" s="14" t="s">
+      <c r="L13" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13" s="76">
         <v>10</v>
       </c>
       <c r="N13" s="14">
@@ -2804,37 +2767,37 @@
       <c r="B14" s="22">
         <v>10</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="77">
         <v>4</v>
       </c>
-      <c r="I14" s="79" t="s">
-        <v>203</v>
-      </c>
-      <c r="J14" s="15" t="s">
+      <c r="I14" s="78" t="s">
+        <v>204</v>
+      </c>
+      <c r="J14" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="L14" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="77">
         <v>10</v>
       </c>
       <c r="N14" s="15">
@@ -2856,37 +2819,37 @@
       <c r="B15" s="2">
         <v>11</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="79" t="s">
+        <v>201</v>
+      </c>
+      <c r="F15" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="79">
+        <v>1</v>
+      </c>
+      <c r="I15" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="3">
-        <v>1</v>
-      </c>
-      <c r="I15" s="77" t="s">
+      <c r="J15" s="79" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="J15" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="M15" s="3">
+      <c r="L15" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15" s="79">
         <v>430</v>
       </c>
       <c r="N15" s="3">
@@ -2904,13 +2867,13 @@
       <c r="R15" s="70"/>
       <c r="S15" s="70"/>
       <c r="T15" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U15" s="3">
         <v>100</v>
       </c>
       <c r="V15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
@@ -2920,37 +2883,37 @@
       <c r="B16" s="17">
         <v>12</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="E16" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="F16" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G16" s="14" t="s">
+      <c r="H16" s="76">
+        <v>2</v>
+      </c>
+      <c r="I16" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="H16" s="14">
-        <v>2</v>
-      </c>
-      <c r="I16" s="72" t="s">
+      <c r="J16" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="J16" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="M16" s="14">
+      <c r="L16" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="M16" s="76">
         <v>20</v>
       </c>
       <c r="N16" s="14">
@@ -2968,13 +2931,13 @@
       <c r="R16" s="71"/>
       <c r="S16" s="71"/>
       <c r="T16" s="41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="U16" s="27">
         <v>40</v>
       </c>
       <c r="V16" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
@@ -2984,37 +2947,37 @@
       <c r="B17" s="17">
         <v>13</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="14" t="s">
+      <c r="C17" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="76" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="76" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="76" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="14" t="s">
+      <c r="H17" s="76">
+        <v>2</v>
+      </c>
+      <c r="I17" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="H17" s="14">
-        <v>2</v>
-      </c>
-      <c r="I17" s="72" t="s">
+      <c r="J17" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="76" t="s">
         <v>73</v>
       </c>
-      <c r="J17" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="L17" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="M17" s="14">
+      <c r="L17" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="M17" s="76">
         <v>30</v>
       </c>
       <c r="N17" s="14">
@@ -3032,13 +2995,13 @@
       <c r="R17" s="71"/>
       <c r="S17" s="71"/>
       <c r="T17" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U17" s="27">
         <v>20</v>
       </c>
       <c r="V17" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
@@ -3048,37 +3011,37 @@
       <c r="B18" s="17">
         <v>14</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="14" t="s">
+      <c r="C18" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="76" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="14" t="s">
+      <c r="H18" s="76">
+        <v>1</v>
+      </c>
+      <c r="I18" s="76" t="s">
+        <v>202</v>
+      </c>
+      <c r="J18" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="H18" s="14">
-        <v>1</v>
-      </c>
-      <c r="I18" s="72" t="s">
-        <v>205</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K18" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="L18" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="M18" s="14">
+      <c r="L18" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="M18" s="76">
         <v>20</v>
       </c>
       <c r="N18" s="14">
@@ -3096,13 +3059,13 @@
       <c r="R18" s="71"/>
       <c r="S18" s="71"/>
       <c r="T18" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U18" s="27">
         <v>40</v>
       </c>
       <c r="V18" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
@@ -3112,35 +3075,35 @@
       <c r="B19" s="17">
         <v>15</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="14" t="s">
+      <c r="F19" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76">
+        <v>5</v>
+      </c>
+      <c r="I19" s="80" t="s">
+        <v>205</v>
+      </c>
+      <c r="J19" s="76" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="F19" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14">
-        <v>5</v>
-      </c>
-      <c r="I19" s="78" t="s">
-        <v>204</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="K19" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="L19" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="M19" s="14">
+      <c r="L19" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="M19" s="76">
         <v>60</v>
       </c>
       <c r="N19" s="14">
@@ -3158,13 +3121,13 @@
       <c r="R19" s="71"/>
       <c r="S19" s="71"/>
       <c r="T19" s="43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U19" s="27">
         <v>120</v>
       </c>
       <c r="V19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
@@ -3174,37 +3137,37 @@
       <c r="B20" s="17">
         <v>16</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="76" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="76" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="14" t="s">
+      <c r="F20" s="76" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="F20" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="G20" s="14" t="s">
+      <c r="H20" s="76">
+        <v>1</v>
+      </c>
+      <c r="I20" s="76" t="s">
         <v>84</v>
       </c>
-      <c r="H20" s="14">
-        <v>1</v>
-      </c>
-      <c r="I20" s="14" t="s">
+      <c r="J20" s="76" t="s">
+        <v>86</v>
+      </c>
+      <c r="K20" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="J20" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="K20" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="L20" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="M20" s="14">
+      <c r="L20" s="76" t="s">
+        <v>81</v>
+      </c>
+      <c r="M20" s="76">
         <v>2760</v>
       </c>
       <c r="N20" s="14">
@@ -3222,13 +3185,13 @@
       <c r="R20" s="71"/>
       <c r="S20" s="71"/>
       <c r="T20" s="41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U20" s="27">
         <v>40</v>
       </c>
       <c r="V20" s="35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
@@ -3238,37 +3201,37 @@
       <c r="B21" s="17">
         <v>17</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="76" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="76" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" s="14" t="s">
+      <c r="F21" s="76" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" s="14" t="s">
+      <c r="H21" s="76">
+        <v>1</v>
+      </c>
+      <c r="I21" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="H21" s="14">
-        <v>1</v>
-      </c>
-      <c r="I21" s="72" t="s">
+      <c r="J21" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21" s="76" t="s">
         <v>91</v>
       </c>
-      <c r="J21" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="K21" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="L21" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="M21" s="14">
+      <c r="L21" s="76" t="s">
+        <v>87</v>
+      </c>
+      <c r="M21" s="76">
         <v>1170</v>
       </c>
       <c r="N21" s="14">
@@ -3286,13 +3249,13 @@
       <c r="R21" s="71"/>
       <c r="S21" s="71"/>
       <c r="T21" s="41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="U21" s="27">
         <v>60</v>
       </c>
       <c r="V21" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
@@ -3302,37 +3265,37 @@
       <c r="B22" s="17">
         <v>18</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="76" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="14" t="s">
+      <c r="H22" s="76">
+        <v>1</v>
+      </c>
+      <c r="I22" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="H22" s="14">
-        <v>1</v>
-      </c>
-      <c r="I22" s="72" t="s">
+      <c r="J22" s="76" t="s">
+        <v>97</v>
+      </c>
+      <c r="K22" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="J22" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="K22" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="M22" s="14">
+      <c r="L22" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="M22" s="76">
         <v>870</v>
       </c>
       <c r="N22" s="14">
@@ -3350,13 +3313,13 @@
       <c r="R22" s="71"/>
       <c r="S22" s="71"/>
       <c r="T22" s="41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="U22" s="27">
         <v>40</v>
       </c>
       <c r="V22" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
@@ -3366,37 +3329,37 @@
       <c r="B23" s="17">
         <v>19</v>
       </c>
-      <c r="C23" s="72" t="s">
-        <v>198</v>
-      </c>
-      <c r="D23" s="72" t="s">
-        <v>198</v>
-      </c>
-      <c r="E23" s="72" t="s">
+      <c r="C23" s="76" t="s">
+        <v>197</v>
+      </c>
+      <c r="D23" s="76" t="s">
+        <v>197</v>
+      </c>
+      <c r="E23" s="76" t="s">
+        <v>195</v>
+      </c>
+      <c r="F23" s="76" t="s">
+        <v>197</v>
+      </c>
+      <c r="G23" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="F23" s="72" t="s">
-        <v>198</v>
-      </c>
-      <c r="G23" s="72" t="s">
+      <c r="H23" s="76">
+        <v>1</v>
+      </c>
+      <c r="I23" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="J23" s="76" t="s">
+        <v>100</v>
+      </c>
+      <c r="K23" s="76" t="s">
+        <v>99</v>
+      </c>
+      <c r="L23" s="76" t="s">
         <v>197</v>
       </c>
-      <c r="H23" s="14">
-        <v>1</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="K23" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="L23" s="72" t="s">
-        <v>198</v>
-      </c>
-      <c r="M23" s="72">
+      <c r="M23" s="76">
         <v>30</v>
       </c>
       <c r="N23" s="14">
@@ -3421,7 +3384,7 @@
         <v>300</v>
       </c>
       <c r="T23" s="69" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="U23" s="27"/>
     </row>
@@ -3432,37 +3395,37 @@
       <c r="B24" s="17">
         <v>20</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="14" t="s">
+      <c r="F24" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="F24" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="G24" s="14" t="s">
+      <c r="H24" s="76">
+        <v>1</v>
+      </c>
+      <c r="I24" s="76" t="s">
         <v>104</v>
       </c>
-      <c r="H24" s="14">
-        <v>1</v>
-      </c>
-      <c r="I24" s="14" t="s">
+      <c r="J24" s="76" t="s">
+        <v>106</v>
+      </c>
+      <c r="K24" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="J24" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="K24" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="L24" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="M24" s="14">
+      <c r="L24" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="M24" s="76">
         <v>50</v>
       </c>
       <c r="N24" s="14">
@@ -3487,7 +3450,7 @@
         <v>5000</v>
       </c>
       <c r="T24" s="69" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="U24" s="27"/>
     </row>
@@ -3498,37 +3461,37 @@
       <c r="B25" s="17">
         <v>21</v>
       </c>
-      <c r="C25" s="72" t="s">
-        <v>199</v>
-      </c>
-      <c r="D25" s="72" t="s">
-        <v>199</v>
-      </c>
-      <c r="E25" s="72" t="s">
-        <v>196</v>
-      </c>
-      <c r="F25" s="72" t="s">
-        <v>199</v>
-      </c>
-      <c r="G25" s="72" t="s">
+      <c r="C25" s="76" t="s">
+        <v>198</v>
+      </c>
+      <c r="D25" s="76" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" s="76" t="s">
         <v>195</v>
       </c>
-      <c r="H25" s="14">
+      <c r="F25" s="76" t="s">
+        <v>198</v>
+      </c>
+      <c r="G25" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="H25" s="76">
         <v>2</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="I25" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="J25" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="K25" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="J25" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="K25" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="L25" s="72" t="s">
-        <v>199</v>
-      </c>
-      <c r="M25" s="72">
+      <c r="L25" s="76" t="s">
+        <v>198</v>
+      </c>
+      <c r="M25" s="76">
         <v>290</v>
       </c>
       <c r="N25" s="14">
@@ -3553,7 +3516,7 @@
         <v>5800</v>
       </c>
       <c r="T25" s="69" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U25" s="27"/>
     </row>
@@ -3564,37 +3527,37 @@
       <c r="B26" s="17">
         <v>22</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="76" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="E26" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="F26" s="76" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="F26" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="G26" s="14" t="s">
+      <c r="H26" s="76">
+        <v>1</v>
+      </c>
+      <c r="I26" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="H26" s="14">
-        <v>1</v>
-      </c>
-      <c r="I26" s="72" t="s">
+      <c r="J26" s="76" t="s">
+        <v>116</v>
+      </c>
+      <c r="K26" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="J26" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="K26" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="L26" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="M26" s="14">
+      <c r="L26" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="M26" s="76">
         <v>100</v>
       </c>
       <c r="N26" s="14">
@@ -3619,7 +3582,7 @@
         <v>1000</v>
       </c>
       <c r="T26" s="69" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U26" s="27"/>
     </row>
@@ -3630,37 +3593,37 @@
       <c r="B27" s="17">
         <v>23</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="76" t="s">
+        <v>199</v>
+      </c>
+      <c r="D27" s="76" t="s">
         <v>200</v>
       </c>
-      <c r="D27" s="72" t="s">
-        <v>201</v>
-      </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="76" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" s="76" t="s">
+        <v>192</v>
+      </c>
+      <c r="G27" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="F27" s="72" t="s">
-        <v>193</v>
-      </c>
-      <c r="G27" s="14" t="s">
+      <c r="H27" s="76">
+        <v>1</v>
+      </c>
+      <c r="I27" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="H27" s="14">
-        <v>1</v>
-      </c>
-      <c r="I27" s="40" t="s">
+      <c r="J27" s="76" t="s">
+        <v>122</v>
+      </c>
+      <c r="K27" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="J27" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="K27" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="L27" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="M27" s="72">
+      <c r="L27" s="76" t="s">
+        <v>117</v>
+      </c>
+      <c r="M27" s="76">
         <v>430</v>
       </c>
       <c r="N27" s="14">
@@ -3685,7 +3648,7 @@
         <v>4300</v>
       </c>
       <c r="T27" s="69" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="U27" s="27"/>
     </row>
@@ -3696,37 +3659,37 @@
       <c r="B28" s="17">
         <v>24</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" s="76" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="G28" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="D28" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="G28" s="14" t="s">
+      <c r="H28" s="76">
+        <v>1</v>
+      </c>
+      <c r="I28" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="H28" s="14">
-        <v>1</v>
-      </c>
-      <c r="I28" s="40" t="s">
+      <c r="J28" s="76" t="s">
+        <v>127</v>
+      </c>
+      <c r="K28" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="J28" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="K28" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L28" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="M28" s="72">
+      <c r="L28" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="M28" s="76">
         <v>430</v>
       </c>
       <c r="N28" s="14">
@@ -3751,7 +3714,7 @@
         <v>4300</v>
       </c>
       <c r="T28" s="69" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="U28" s="27"/>
     </row>
@@ -3833,7 +3796,7 @@
         <v>6</v>
       </c>
       <c r="I30" s="38" t="s">
-        <v>54</v>
+        <v>203</v>
       </c>
       <c r="J30" s="38" t="s">
         <v>20</v>
@@ -3871,7 +3834,7 @@
     </row>
     <row r="32" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U32" s="26"/>
     </row>
@@ -3900,21 +3863,21 @@
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
+        <v>167</v>
+      </c>
+      <c r="J3" s="59" t="s">
         <v>168</v>
-      </c>
-      <c r="J3" s="59" t="s">
-        <v>169</v>
       </c>
       <c r="K3" s="68"/>
       <c r="L3" s="68"/>
       <c r="M3" s="68"/>
       <c r="O3" s="59" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P3" s="68"/>
       <c r="Q3" s="68"/>
@@ -3922,45 +3885,45 @@
     </row>
     <row r="4" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="45" t="s">
         <v>150</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="E4" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="F4" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="F4" s="46" t="s">
-        <v>153</v>
-      </c>
       <c r="J4" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="K4" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="L4" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="L4" s="45" t="s">
+      <c r="M4" s="46" t="s">
         <v>172</v>
       </c>
-      <c r="M4" s="46" t="s">
-        <v>173</v>
-      </c>
       <c r="O4" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="P4" s="45" t="s">
         <v>181</v>
       </c>
-      <c r="P4" s="45" t="s">
+      <c r="Q4" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="Q4" s="45" t="s">
+      <c r="R4" s="46" t="s">
         <v>183</v>
-      </c>
-      <c r="R4" s="46" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C5" s="47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="48">
         <v>52</v>
@@ -3973,7 +3936,7 @@
         <v>34840</v>
       </c>
       <c r="J5" s="47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K5" s="48">
         <v>169</v>
@@ -3986,7 +3949,7 @@
         <v>84500</v>
       </c>
       <c r="O5" s="47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P5" s="48">
         <v>169</v>
@@ -4001,39 +3964,39 @@
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C6" s="50" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D6" s="51">
         <v>15</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F6" s="53">
         <f>F5*D6/100</f>
         <v>5226</v>
       </c>
       <c r="J6" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K6" s="51">
         <v>15</v>
       </c>
       <c r="L6" s="52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M6" s="53">
         <f>M5*K6/100</f>
         <v>12675</v>
       </c>
       <c r="O6" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P6" s="51">
         <v>15</v>
       </c>
       <c r="Q6" s="52" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="R6" s="53">
         <f>R5*P6/100</f>
@@ -4042,39 +4005,39 @@
     </row>
     <row r="7" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="54" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D7" s="55">
         <v>15</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F7" s="57">
         <f>F5*D7/100</f>
         <v>5226</v>
       </c>
       <c r="J7" s="54" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K7" s="55">
         <v>0</v>
       </c>
       <c r="L7" s="56" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M7" s="57">
         <f>M5*K7/100</f>
         <v>0</v>
       </c>
       <c r="O7" s="54" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P7" s="55">
         <v>15</v>
       </c>
       <c r="Q7" s="56" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R7" s="57">
         <f>R5*P7/100</f>
@@ -4082,29 +4045,29 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="73" t="s">
-        <v>158</v>
-      </c>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
+      <c r="C8" s="72" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="58">
         <f>SUM(F5:F7)</f>
         <v>45292</v>
       </c>
-      <c r="J8" s="73" t="s">
-        <v>158</v>
-      </c>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
+      <c r="J8" s="72" t="s">
+        <v>157</v>
+      </c>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
       <c r="M8" s="58">
         <f>SUM(M5:M7)</f>
         <v>97175</v>
       </c>
-      <c r="O8" s="73" t="s">
-        <v>158</v>
-      </c>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="74"/>
+      <c r="O8" s="72" t="s">
+        <v>157</v>
+      </c>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
       <c r="R8" s="58">
         <f>SUM(R5:R7)</f>
         <v>138411</v>
@@ -4126,45 +4089,45 @@
     </row>
     <row r="10" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="62" t="s">
         <v>159</v>
       </c>
-      <c r="D10" s="62" t="s">
+      <c r="E10" s="63" t="s">
         <v>160</v>
       </c>
-      <c r="E10" s="63" t="s">
+      <c r="F10" s="64" t="s">
         <v>161</v>
       </c>
-      <c r="F10" s="64" t="s">
-        <v>162</v>
-      </c>
       <c r="J10" s="61" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K10" s="62" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L10" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="M10" s="64" t="s">
         <v>172</v>
       </c>
-      <c r="M10" s="64" t="s">
-        <v>173</v>
-      </c>
       <c r="O10" s="61" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P10" s="62" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q10" s="63" t="s">
+        <v>182</v>
+      </c>
+      <c r="R10" s="64" t="s">
         <v>183</v>
-      </c>
-      <c r="R10" s="64" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C11" s="47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D11" s="48">
         <v>100</v>
@@ -4178,7 +4141,7 @@
         <v>4529200</v>
       </c>
       <c r="J11" s="47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K11" s="48">
         <v>4</v>
@@ -4192,7 +4155,7 @@
         <v>388700</v>
       </c>
       <c r="O11" s="47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P11" s="48">
         <v>4</v>
@@ -4208,7 +4171,7 @@
     </row>
     <row r="12" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="54" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D12" s="66">
         <v>1</v>
@@ -4221,7 +4184,7 @@
         <v>110000</v>
       </c>
       <c r="J12" s="54" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K12" s="66">
         <v>4</v>
@@ -4234,7 +4197,7 @@
         <v>0</v>
       </c>
       <c r="O12" s="54" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P12" s="66">
         <v>4</v>
@@ -4249,7 +4212,7 @@
     </row>
     <row r="13" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="54" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D13" s="66">
         <v>100</v>
@@ -4262,61 +4225,61 @@
         <f>D13*E13</f>
         <v>798000</v>
       </c>
-      <c r="J13" s="73" t="s">
-        <v>179</v>
-      </c>
-      <c r="K13" s="74"/>
-      <c r="L13" s="75">
+      <c r="J13" s="72" t="s">
+        <v>178</v>
+      </c>
+      <c r="K13" s="73"/>
+      <c r="L13" s="74">
         <f>M11</f>
         <v>388700</v>
       </c>
-      <c r="M13" s="76"/>
-      <c r="O13" s="73" t="s">
-        <v>179</v>
-      </c>
-      <c r="P13" s="74"/>
-      <c r="Q13" s="75">
+      <c r="M13" s="75"/>
+      <c r="O13" s="72" t="s">
+        <v>178</v>
+      </c>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="74">
         <f>R11</f>
         <v>553644</v>
       </c>
-      <c r="R13" s="76"/>
+      <c r="R13" s="75"/>
     </row>
     <row r="14" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="73" t="s">
-        <v>165</v>
-      </c>
-      <c r="D14" s="74"/>
-      <c r="E14" s="75">
+      <c r="C14" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="D14" s="73"/>
+      <c r="E14" s="74">
         <f>SUM(F11:F13)</f>
         <v>5437200</v>
       </c>
-      <c r="F14" s="76"/>
+      <c r="F14" s="75"/>
     </row>
     <row r="15" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="73" t="s">
-        <v>167</v>
-      </c>
-      <c r="D16" s="74"/>
-      <c r="E16" s="75">
+      <c r="C16" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" s="73"/>
+      <c r="E16" s="74">
         <f>E14/D11</f>
         <v>54372</v>
       </c>
-      <c r="F16" s="76"/>
+      <c r="F16" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="O13:P13"/>
     <mergeCell ref="Q13:R13"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>